<commit_message>
Made some formatting changes
</commit_message>
<xml_diff>
--- a/T04_M3_D2_Dimension_Mapping_files/T04_M3_D2_Dimension_Mapping_metadata.xlsx
+++ b/T04_M3_D2_Dimension_Mapping_files/T04_M3_D2_Dimension_Mapping_metadata.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\New folder (3)\Course Material UST\Sem 5-Spr2018\Data Warehousing\Project\M3\Answers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\New folder (3)\Course Material UST\Sem 5-Spr2018\Data Warehousing\Project\M3\Answers\T04_M3_D2_Dimension_Mapping_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE06465-92FF-4DDD-B17B-C713B4279802}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E19108-1492-45EF-AE63-AF69F6725644}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="4" xr2:uid="{4BCD3B06-A9D7-4471-91C7-2D4ACC75E743}"/>
   </bookViews>
   <sheets>
     <sheet name="MSA" sheetId="1" r:id="rId1"/>
-    <sheet name="Package" sheetId="2" r:id="rId2"/>
-    <sheet name="Product" sheetId="3" r:id="rId3"/>
-    <sheet name="Purchase_Date" sheetId="4" r:id="rId4"/>
-    <sheet name="Sales_Org" sheetId="5" r:id="rId5"/>
+    <sheet name="PACKAGE" sheetId="2" r:id="rId2"/>
+    <sheet name="PRODUCT" sheetId="3" r:id="rId3"/>
+    <sheet name="PURCHASE_DATE" sheetId="4" r:id="rId4"/>
+    <sheet name="SALES_ORG" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -112,9 +112,6 @@
     <t>MSA_Metropolitan_Area_Key</t>
   </si>
   <si>
-    <t>Package</t>
-  </si>
-  <si>
     <t>PKG_Key</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>FEA_Value</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>PRD_Key</t>
   </si>
   <si>
@@ -301,9 +295,6 @@
     <t>MMC_ID</t>
   </si>
   <si>
-    <t>Purchase_Date</t>
-  </si>
-  <si>
     <t>PDAT_Key</t>
   </si>
   <si>
@@ -455,6 +446,15 @@
   </si>
   <si>
     <t>PDAT_Day_Of_Quarter</t>
+  </si>
+  <si>
+    <t>PACKAGE</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>PURCHASE_DATE</t>
   </si>
 </sst>
 </file>
@@ -968,33 +968,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1013,38 +986,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1061,45 +1004,129 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1107,33 +1134,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1467,62 +1467,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="46" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="59" t="s">
+      <c r="L2" s="40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1536,11 +1536,11 @@
       <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="69"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
@@ -1549,30 +1549,30 @@
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="61"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1601,30 +1601,30 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="23" t="s">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="61"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1653,30 +1653,30 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="61"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1705,26 +1705,26 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1758,62 +1758,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="67" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="71" t="s">
+      <c r="H2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="59" t="s">
+      <c r="L2" s="40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1822,67 +1822,67 @@
         <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="72"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="81"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="51"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="31" t="s">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="F4" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="61"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
@@ -1892,576 +1892,576 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="32" t="s">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="G6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="61"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="32" t="s">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="G8" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" s="60"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="61"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="32" t="s">
+      <c r="A10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="G10" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="60"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="61"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="32" t="s">
+      <c r="A12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="G12" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="60"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="61"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="32" t="s">
+      <c r="A14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="G14" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="60"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="61"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="32" t="s">
+      <c r="A16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="G16" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J16" s="60"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="61"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="42"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="32" t="s">
+      <c r="A18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="G18" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="60"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="61"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="42"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="32" t="s">
+      <c r="A20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="G20" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J20" s="60"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="61"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="32" t="s">
+      <c r="A22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="G22" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="I22" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="60"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="61"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="42"/>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="G23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="5"/>
@@ -2484,7 +2484,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B4" sqref="B4:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2498,62 +2498,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="46" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="59" t="s">
+      <c r="L2" s="40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2562,16 +2562,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="69"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
@@ -2580,45 +2580,45 @@
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="61"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
@@ -2628,46 +2628,46 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="32" t="s">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="61"/>
+      <c r="D6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="3"/>
@@ -2676,49 +2676,49 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="61"/>
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="33"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
@@ -2728,45 +2728,45 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="76" t="s">
+      <c r="A10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="77"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="61"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
@@ -2776,46 +2776,46 @@
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="52"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="61"/>
+      <c r="A12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="33"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="75"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
       <c r="I13" s="3"/>
@@ -2824,49 +2824,49 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="A14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="61"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1"/>
@@ -2876,49 +2876,49 @@
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="61"/>
+      <c r="A16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="42"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="1"/>
@@ -2928,49 +2928,49 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="32" t="s">
+      <c r="A18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="61"/>
+      <c r="D18" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="42"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="1"/>
@@ -2980,49 +2980,49 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="61"/>
+      <c r="A20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -3033,15 +3033,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3052,7 +3052,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B4" sqref="B4:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3066,62 +3066,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="46" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="59" t="s">
+      <c r="L2" s="40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3130,10 +3130,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>10</v>
@@ -3148,40 +3148,40 @@
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="61"/>
+      <c r="F4" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -3196,49 +3196,49 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="23" t="s">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="61"/>
+      <c r="F6" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
@@ -3248,49 +3248,49 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="61"/>
+      <c r="F8" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="33"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
@@ -3300,49 +3300,49 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="52"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="61"/>
+      <c r="F10" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="33"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
@@ -3352,45 +3352,45 @@
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="31" t="s">
+      <c r="A12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="61"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
@@ -3400,49 +3400,49 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="61"/>
+      <c r="F14" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1"/>
@@ -3452,49 +3452,49 @@
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="23" t="s">
+      <c r="A16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="61"/>
+      <c r="F16" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="42"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F17" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="1"/>
@@ -3504,49 +3504,49 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="23" t="s">
+      <c r="A18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="61"/>
+      <c r="F18" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="42"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="1"/>
@@ -3556,49 +3556,49 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="61"/>
+      <c r="F20" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F21" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="1"/>
@@ -3608,30 +3608,30 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="63"/>
-      <c r="L22" s="64"/>
+      <c r="F22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3665,62 +3665,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="91" t="s">
+      <c r="E1" s="86"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="92"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="82" t="s">
+      <c r="H1" s="89"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="83"/>
-      <c r="L1" s="84"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="93"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="71" t="s">
+      <c r="H2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="59" t="s">
+      <c r="L2" s="40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3729,16 +3729,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="69"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
@@ -3747,49 +3747,49 @@
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="61"/>
+      <c r="F4" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
@@ -3799,52 +3799,52 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="G6" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="61"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="3"/>
@@ -3853,49 +3853,49 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="31" t="s">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="61"/>
+      <c r="E8" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="33"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
@@ -3905,55 +3905,55 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="31" t="s">
+      <c r="A10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10" s="52" t="s">
+      <c r="E10" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="I10" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="J10" s="60"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="61"/>
+      <c r="H10" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="41"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
@@ -3963,121 +3963,121 @@
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="31" t="s">
+      <c r="A12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="G12" s="52"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="61"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="76" t="s">
+      <c r="A14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="77"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="61"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>